<commit_message>
Another Change has been made
</commit_message>
<xml_diff>
--- a/Excel1.xlsx
+++ b/Excel1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aparna\Documents\Git Practice\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aparna\Documents\Git_Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F4418E-6F48-4DC4-B574-4580BC537BCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD7C3550-250B-462A-9E4B-7C8D3FF82284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,19 +25,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>1st change</t>
   </si>
+  <si>
+    <t>2nd change</t>
+  </si>
+  <si>
+    <t>3rd change</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -345,20 +357,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>